<commit_message>
Uploading new data files: body weight and density part 1 egg data.
</commit_message>
<xml_diff>
--- a/data/fitness_development/bodyweight_flies.xlsx
+++ b/data/fitness_development/bodyweight_flies.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster_12/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster_13/data/fitness_development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C5D9BFB-DCA9-8D43-8780-10AC6877F24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A4C371-D613-B647-974F-111644D2CA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{7076ED54-3A1B-1840-8818-465FA310ADBC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="8">
   <si>
     <t>treatment</t>
   </si>
@@ -431,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E0960C-F631-A24B-86EC-5117F5F33DB5}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D221"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F97" sqref="F97"/>
+    <sheetView tabSelected="1" topLeftCell="A170" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D220" sqref="D220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1857,6 +1857,1677 @@
         <v>0.51200000000000001</v>
       </c>
     </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>4</v>
+      </c>
+      <c r="B102" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+      <c r="D102">
+        <v>0.23200000000000001</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>4</v>
+      </c>
+      <c r="B103" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
+      </c>
+      <c r="D103">
+        <v>0.40799999999999997</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>4</v>
+      </c>
+      <c r="B104" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104">
+        <v>3</v>
+      </c>
+      <c r="D104">
+        <v>0.44800000000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>4</v>
+      </c>
+      <c r="B105" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105">
+        <v>4</v>
+      </c>
+      <c r="D105">
+        <v>0.31900000000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>4</v>
+      </c>
+      <c r="B106" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106">
+        <v>5</v>
+      </c>
+      <c r="D106">
+        <v>0.36899999999999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>4</v>
+      </c>
+      <c r="B107" t="s">
+        <v>6</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+      <c r="D107">
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>4</v>
+      </c>
+      <c r="B108" t="s">
+        <v>6</v>
+      </c>
+      <c r="C108">
+        <v>2</v>
+      </c>
+      <c r="D108">
+        <v>0.57099999999999995</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>4</v>
+      </c>
+      <c r="B109" t="s">
+        <v>6</v>
+      </c>
+      <c r="C109">
+        <v>3</v>
+      </c>
+      <c r="D109">
+        <v>0.56799999999999995</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>4</v>
+      </c>
+      <c r="B110" t="s">
+        <v>6</v>
+      </c>
+      <c r="C110">
+        <v>4</v>
+      </c>
+      <c r="D110">
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>4</v>
+      </c>
+      <c r="B111" t="s">
+        <v>6</v>
+      </c>
+      <c r="C111">
+        <v>5</v>
+      </c>
+      <c r="D111">
+        <v>0.56899999999999995</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>7</v>
+      </c>
+      <c r="B112" t="s">
+        <v>5</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+      <c r="D112">
+        <v>0.46400000000000002</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>7</v>
+      </c>
+      <c r="B113" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113">
+        <v>2</v>
+      </c>
+      <c r="D113">
+        <v>0.38200000000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>7</v>
+      </c>
+      <c r="B114" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114">
+        <v>3</v>
+      </c>
+      <c r="D114">
+        <v>0.19800000000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>7</v>
+      </c>
+      <c r="B115" t="s">
+        <v>5</v>
+      </c>
+      <c r="C115">
+        <v>4</v>
+      </c>
+      <c r="D115">
+        <v>0.32400000000000001</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>7</v>
+      </c>
+      <c r="B116" t="s">
+        <v>5</v>
+      </c>
+      <c r="C116">
+        <v>5</v>
+      </c>
+      <c r="D116">
+        <v>0.438</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>7</v>
+      </c>
+      <c r="B117" t="s">
+        <v>6</v>
+      </c>
+      <c r="C117">
+        <v>1</v>
+      </c>
+      <c r="D117">
+        <v>0.49099999999999999</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>7</v>
+      </c>
+      <c r="B118" t="s">
+        <v>6</v>
+      </c>
+      <c r="C118">
+        <v>2</v>
+      </c>
+      <c r="D118">
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>7</v>
+      </c>
+      <c r="B119" t="s">
+        <v>6</v>
+      </c>
+      <c r="C119">
+        <v>3</v>
+      </c>
+      <c r="D119">
+        <v>0.54700000000000004</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>7</v>
+      </c>
+      <c r="B120" t="s">
+        <v>6</v>
+      </c>
+      <c r="C120">
+        <v>4</v>
+      </c>
+      <c r="D120">
+        <v>0.47799999999999998</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>7</v>
+      </c>
+      <c r="B121" t="s">
+        <v>6</v>
+      </c>
+      <c r="C121">
+        <v>5</v>
+      </c>
+      <c r="D121">
+        <v>0.55300000000000005</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>4</v>
+      </c>
+      <c r="B122" t="s">
+        <v>5</v>
+      </c>
+      <c r="C122">
+        <v>1</v>
+      </c>
+      <c r="D122">
+        <v>0.40699999999999997</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>4</v>
+      </c>
+      <c r="B123" t="s">
+        <v>5</v>
+      </c>
+      <c r="C123">
+        <v>2</v>
+      </c>
+      <c r="D123">
+        <v>0.41899999999999998</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>4</v>
+      </c>
+      <c r="B124" t="s">
+        <v>5</v>
+      </c>
+      <c r="C124">
+        <v>3</v>
+      </c>
+      <c r="D124">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>4</v>
+      </c>
+      <c r="B125" t="s">
+        <v>5</v>
+      </c>
+      <c r="C125">
+        <v>4</v>
+      </c>
+      <c r="D125">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>4</v>
+      </c>
+      <c r="B126" t="s">
+        <v>5</v>
+      </c>
+      <c r="C126">
+        <v>5</v>
+      </c>
+      <c r="D126">
+        <v>0.38600000000000001</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>4</v>
+      </c>
+      <c r="B127" t="s">
+        <v>6</v>
+      </c>
+      <c r="C127">
+        <v>1</v>
+      </c>
+      <c r="D127">
+        <v>0.51100000000000001</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>4</v>
+      </c>
+      <c r="B128" t="s">
+        <v>6</v>
+      </c>
+      <c r="C128">
+        <v>2</v>
+      </c>
+      <c r="D128">
+        <v>0.377</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>4</v>
+      </c>
+      <c r="B129" t="s">
+        <v>6</v>
+      </c>
+      <c r="C129">
+        <v>3</v>
+      </c>
+      <c r="D129">
+        <v>0.38200000000000001</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>4</v>
+      </c>
+      <c r="B130" t="s">
+        <v>6</v>
+      </c>
+      <c r="C130">
+        <v>4</v>
+      </c>
+      <c r="D130">
+        <v>0.45900000000000002</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>4</v>
+      </c>
+      <c r="B131" t="s">
+        <v>6</v>
+      </c>
+      <c r="C131">
+        <v>5</v>
+      </c>
+      <c r="D131">
+        <v>0.51500000000000001</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>7</v>
+      </c>
+      <c r="B132" t="s">
+        <v>5</v>
+      </c>
+      <c r="C132">
+        <v>1</v>
+      </c>
+      <c r="D132">
+        <v>0.435</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>7</v>
+      </c>
+      <c r="B133" t="s">
+        <v>5</v>
+      </c>
+      <c r="C133">
+        <v>2</v>
+      </c>
+      <c r="D133">
+        <v>0.38300000000000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>7</v>
+      </c>
+      <c r="B134" t="s">
+        <v>5</v>
+      </c>
+      <c r="C134">
+        <v>3</v>
+      </c>
+      <c r="D134">
+        <v>0.33200000000000002</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>7</v>
+      </c>
+      <c r="B135" t="s">
+        <v>5</v>
+      </c>
+      <c r="C135">
+        <v>4</v>
+      </c>
+      <c r="D135">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>7</v>
+      </c>
+      <c r="B136" t="s">
+        <v>5</v>
+      </c>
+      <c r="C136">
+        <v>5</v>
+      </c>
+      <c r="D136">
+        <v>0.46400000000000002</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>7</v>
+      </c>
+      <c r="B137" t="s">
+        <v>6</v>
+      </c>
+      <c r="C137">
+        <v>1</v>
+      </c>
+      <c r="D137">
+        <v>0.54400000000000004</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>7</v>
+      </c>
+      <c r="B138" t="s">
+        <v>6</v>
+      </c>
+      <c r="C138">
+        <v>2</v>
+      </c>
+      <c r="D138">
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>7</v>
+      </c>
+      <c r="B139" t="s">
+        <v>6</v>
+      </c>
+      <c r="C139">
+        <v>3</v>
+      </c>
+      <c r="D139">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>7</v>
+      </c>
+      <c r="B140" t="s">
+        <v>6</v>
+      </c>
+      <c r="C140">
+        <v>4</v>
+      </c>
+      <c r="D140">
+        <v>0.505</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>7</v>
+      </c>
+      <c r="B141" t="s">
+        <v>6</v>
+      </c>
+      <c r="C141">
+        <v>5</v>
+      </c>
+      <c r="D141">
+        <v>0.438</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>4</v>
+      </c>
+      <c r="B142" t="s">
+        <v>5</v>
+      </c>
+      <c r="C142">
+        <v>1</v>
+      </c>
+      <c r="D142">
+        <v>0.45300000000000001</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>4</v>
+      </c>
+      <c r="B143" t="s">
+        <v>5</v>
+      </c>
+      <c r="C143">
+        <v>2</v>
+      </c>
+      <c r="D143">
+        <v>0.41599999999999998</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>4</v>
+      </c>
+      <c r="B144" t="s">
+        <v>5</v>
+      </c>
+      <c r="C144">
+        <v>3</v>
+      </c>
+      <c r="D144">
+        <v>0.48099999999999998</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>4</v>
+      </c>
+      <c r="B145" t="s">
+        <v>5</v>
+      </c>
+      <c r="C145">
+        <v>4</v>
+      </c>
+      <c r="D145">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>4</v>
+      </c>
+      <c r="B146" t="s">
+        <v>5</v>
+      </c>
+      <c r="C146">
+        <v>5</v>
+      </c>
+      <c r="D146">
+        <v>0.39300000000000002</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>4</v>
+      </c>
+      <c r="B147" t="s">
+        <v>6</v>
+      </c>
+      <c r="C147">
+        <v>1</v>
+      </c>
+      <c r="D147">
+        <v>0.51900000000000002</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>4</v>
+      </c>
+      <c r="B148" t="s">
+        <v>6</v>
+      </c>
+      <c r="C148">
+        <v>2</v>
+      </c>
+      <c r="D148">
+        <v>0.68899999999999995</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>4</v>
+      </c>
+      <c r="B149" t="s">
+        <v>6</v>
+      </c>
+      <c r="C149">
+        <v>3</v>
+      </c>
+      <c r="D149">
+        <v>0.43099999999999999</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>4</v>
+      </c>
+      <c r="B150" t="s">
+        <v>6</v>
+      </c>
+      <c r="C150">
+        <v>4</v>
+      </c>
+      <c r="D150">
+        <v>0.56100000000000005</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>4</v>
+      </c>
+      <c r="B151" t="s">
+        <v>6</v>
+      </c>
+      <c r="C151">
+        <v>5</v>
+      </c>
+      <c r="D151">
+        <v>0.55100000000000005</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>7</v>
+      </c>
+      <c r="B152" t="s">
+        <v>5</v>
+      </c>
+      <c r="C152">
+        <v>1</v>
+      </c>
+      <c r="D152">
+        <v>0.38200000000000001</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>7</v>
+      </c>
+      <c r="B153" t="s">
+        <v>5</v>
+      </c>
+      <c r="C153">
+        <v>2</v>
+      </c>
+      <c r="D153">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>7</v>
+      </c>
+      <c r="B154" t="s">
+        <v>5</v>
+      </c>
+      <c r="C154">
+        <v>3</v>
+      </c>
+      <c r="D154">
+        <v>0.35299999999999998</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>7</v>
+      </c>
+      <c r="B155" t="s">
+        <v>5</v>
+      </c>
+      <c r="C155">
+        <v>4</v>
+      </c>
+      <c r="D155">
+        <v>0.35399999999999998</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>7</v>
+      </c>
+      <c r="B156" t="s">
+        <v>5</v>
+      </c>
+      <c r="C156">
+        <v>5</v>
+      </c>
+      <c r="D156">
+        <v>0.36099999999999999</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>7</v>
+      </c>
+      <c r="B157" t="s">
+        <v>6</v>
+      </c>
+      <c r="C157">
+        <v>1</v>
+      </c>
+      <c r="D157">
+        <v>0.58399999999999996</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>7</v>
+      </c>
+      <c r="B158" t="s">
+        <v>6</v>
+      </c>
+      <c r="C158">
+        <v>2</v>
+      </c>
+      <c r="D158">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>7</v>
+      </c>
+      <c r="B159" t="s">
+        <v>6</v>
+      </c>
+      <c r="C159">
+        <v>3</v>
+      </c>
+      <c r="D159">
+        <v>0.58399999999999996</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>7</v>
+      </c>
+      <c r="B160" t="s">
+        <v>6</v>
+      </c>
+      <c r="C160">
+        <v>4</v>
+      </c>
+      <c r="D160">
+        <v>0.57699999999999996</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>7</v>
+      </c>
+      <c r="B161" t="s">
+        <v>6</v>
+      </c>
+      <c r="C161">
+        <v>5</v>
+      </c>
+      <c r="D161">
+        <v>0.50700000000000001</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>4</v>
+      </c>
+      <c r="B162" t="s">
+        <v>5</v>
+      </c>
+      <c r="C162">
+        <v>1</v>
+      </c>
+      <c r="D162">
+        <v>0.45300000000000001</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>4</v>
+      </c>
+      <c r="B163" t="s">
+        <v>5</v>
+      </c>
+      <c r="C163">
+        <v>2</v>
+      </c>
+      <c r="D163">
+        <v>0.433</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>4</v>
+      </c>
+      <c r="B164" t="s">
+        <v>5</v>
+      </c>
+      <c r="C164">
+        <v>3</v>
+      </c>
+      <c r="D164">
+        <v>0.41899999999999998</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>4</v>
+      </c>
+      <c r="B165" t="s">
+        <v>5</v>
+      </c>
+      <c r="C165">
+        <v>4</v>
+      </c>
+      <c r="D165">
+        <v>0.36599999999999999</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>4</v>
+      </c>
+      <c r="B166" t="s">
+        <v>5</v>
+      </c>
+      <c r="C166">
+        <v>5</v>
+      </c>
+      <c r="D166">
+        <v>0.313</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>4</v>
+      </c>
+      <c r="B167" t="s">
+        <v>6</v>
+      </c>
+      <c r="C167">
+        <v>1</v>
+      </c>
+      <c r="D167">
+        <v>0.624</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>4</v>
+      </c>
+      <c r="B168" t="s">
+        <v>6</v>
+      </c>
+      <c r="C168">
+        <v>2</v>
+      </c>
+      <c r="D168">
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>4</v>
+      </c>
+      <c r="B169" t="s">
+        <v>6</v>
+      </c>
+      <c r="C169">
+        <v>3</v>
+      </c>
+      <c r="D169">
+        <v>0.65800000000000003</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>4</v>
+      </c>
+      <c r="B170" t="s">
+        <v>6</v>
+      </c>
+      <c r="C170">
+        <v>4</v>
+      </c>
+      <c r="D170">
+        <v>0.439</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>4</v>
+      </c>
+      <c r="B171" t="s">
+        <v>6</v>
+      </c>
+      <c r="C171">
+        <v>5</v>
+      </c>
+      <c r="D171">
+        <v>0.49199999999999999</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>7</v>
+      </c>
+      <c r="B172" t="s">
+        <v>5</v>
+      </c>
+      <c r="C172">
+        <v>1</v>
+      </c>
+      <c r="D172">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>7</v>
+      </c>
+      <c r="B173" t="s">
+        <v>5</v>
+      </c>
+      <c r="C173">
+        <v>2</v>
+      </c>
+      <c r="D173">
+        <v>0.437</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>7</v>
+      </c>
+      <c r="B174" t="s">
+        <v>5</v>
+      </c>
+      <c r="C174">
+        <v>3</v>
+      </c>
+      <c r="D174">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>7</v>
+      </c>
+      <c r="B175" t="s">
+        <v>5</v>
+      </c>
+      <c r="C175">
+        <v>4</v>
+      </c>
+      <c r="D175">
+        <v>0.34599999999999997</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>7</v>
+      </c>
+      <c r="B176" t="s">
+        <v>5</v>
+      </c>
+      <c r="C176">
+        <v>5</v>
+      </c>
+      <c r="D176">
+        <v>0.41099999999999998</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>7</v>
+      </c>
+      <c r="B177" t="s">
+        <v>6</v>
+      </c>
+      <c r="C177">
+        <v>1</v>
+      </c>
+      <c r="D177">
+        <v>0.47199999999999998</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>7</v>
+      </c>
+      <c r="B178" t="s">
+        <v>6</v>
+      </c>
+      <c r="C178">
+        <v>2</v>
+      </c>
+      <c r="D178">
+        <v>0.61899999999999999</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>7</v>
+      </c>
+      <c r="B179" t="s">
+        <v>6</v>
+      </c>
+      <c r="C179">
+        <v>3</v>
+      </c>
+      <c r="D179">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>7</v>
+      </c>
+      <c r="B180" t="s">
+        <v>6</v>
+      </c>
+      <c r="C180">
+        <v>4</v>
+      </c>
+      <c r="D180">
+        <v>0.42299999999999999</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>7</v>
+      </c>
+      <c r="B181" t="s">
+        <v>6</v>
+      </c>
+      <c r="C181">
+        <v>5</v>
+      </c>
+      <c r="D181">
+        <v>0.442</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>4</v>
+      </c>
+      <c r="B182" t="s">
+        <v>5</v>
+      </c>
+      <c r="C182">
+        <v>1</v>
+      </c>
+      <c r="D182">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>4</v>
+      </c>
+      <c r="B183" t="s">
+        <v>5</v>
+      </c>
+      <c r="C183">
+        <v>2</v>
+      </c>
+      <c r="D183">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>4</v>
+      </c>
+      <c r="B184" t="s">
+        <v>5</v>
+      </c>
+      <c r="C184">
+        <v>3</v>
+      </c>
+      <c r="D184">
+        <v>0.44600000000000001</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>4</v>
+      </c>
+      <c r="B185" t="s">
+        <v>5</v>
+      </c>
+      <c r="C185">
+        <v>4</v>
+      </c>
+      <c r="D185">
+        <v>0.39400000000000002</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>4</v>
+      </c>
+      <c r="B186" t="s">
+        <v>5</v>
+      </c>
+      <c r="C186">
+        <v>5</v>
+      </c>
+      <c r="D186">
+        <v>0.47199999999999998</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>4</v>
+      </c>
+      <c r="B187" t="s">
+        <v>6</v>
+      </c>
+      <c r="C187">
+        <v>1</v>
+      </c>
+      <c r="D187">
+        <v>0.60599999999999998</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>4</v>
+      </c>
+      <c r="B188" t="s">
+        <v>6</v>
+      </c>
+      <c r="C188">
+        <v>2</v>
+      </c>
+      <c r="D188">
+        <v>0.499</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>4</v>
+      </c>
+      <c r="B189" t="s">
+        <v>6</v>
+      </c>
+      <c r="C189">
+        <v>3</v>
+      </c>
+      <c r="D189">
+        <v>0.623</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>4</v>
+      </c>
+      <c r="B190" t="s">
+        <v>6</v>
+      </c>
+      <c r="C190">
+        <v>4</v>
+      </c>
+      <c r="D190">
+        <v>0.54600000000000004</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>4</v>
+      </c>
+      <c r="B191" t="s">
+        <v>6</v>
+      </c>
+      <c r="C191">
+        <v>5</v>
+      </c>
+      <c r="D191">
+        <v>0.54400000000000004</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>7</v>
+      </c>
+      <c r="B192" t="s">
+        <v>5</v>
+      </c>
+      <c r="C192">
+        <v>1</v>
+      </c>
+      <c r="D192">
+        <v>0.44600000000000001</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>7</v>
+      </c>
+      <c r="B193" t="s">
+        <v>5</v>
+      </c>
+      <c r="C193">
+        <v>2</v>
+      </c>
+      <c r="D193">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>7</v>
+      </c>
+      <c r="B194" t="s">
+        <v>5</v>
+      </c>
+      <c r="C194">
+        <v>3</v>
+      </c>
+      <c r="D194">
+        <v>0.41199999999999998</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>7</v>
+      </c>
+      <c r="B195" t="s">
+        <v>5</v>
+      </c>
+      <c r="C195">
+        <v>4</v>
+      </c>
+      <c r="D195">
+        <v>0.28599999999999998</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>7</v>
+      </c>
+      <c r="B196" t="s">
+        <v>5</v>
+      </c>
+      <c r="C196">
+        <v>5</v>
+      </c>
+      <c r="D196">
+        <v>0.54500000000000004</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>7</v>
+      </c>
+      <c r="B197" t="s">
+        <v>6</v>
+      </c>
+      <c r="C197">
+        <v>1</v>
+      </c>
+      <c r="D197">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>7</v>
+      </c>
+      <c r="B198" t="s">
+        <v>6</v>
+      </c>
+      <c r="C198">
+        <v>2</v>
+      </c>
+      <c r="D198">
+        <v>0.54700000000000004</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>7</v>
+      </c>
+      <c r="B199" t="s">
+        <v>6</v>
+      </c>
+      <c r="C199">
+        <v>3</v>
+      </c>
+      <c r="D199">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>7</v>
+      </c>
+      <c r="B200" t="s">
+        <v>6</v>
+      </c>
+      <c r="C200">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>7</v>
+      </c>
+      <c r="B201" t="s">
+        <v>6</v>
+      </c>
+      <c r="C201">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>4</v>
+      </c>
+      <c r="B202" t="s">
+        <v>5</v>
+      </c>
+      <c r="C202">
+        <v>1</v>
+      </c>
+      <c r="D202">
+        <v>0.35599999999999998</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>4</v>
+      </c>
+      <c r="B203" t="s">
+        <v>5</v>
+      </c>
+      <c r="C203">
+        <v>2</v>
+      </c>
+      <c r="D203">
+        <v>0.371</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>4</v>
+      </c>
+      <c r="B204" t="s">
+        <v>5</v>
+      </c>
+      <c r="C204">
+        <v>3</v>
+      </c>
+      <c r="D204">
+        <v>0.47899999999999998</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>4</v>
+      </c>
+      <c r="B205" t="s">
+        <v>5</v>
+      </c>
+      <c r="C205">
+        <v>4</v>
+      </c>
+      <c r="D205">
+        <v>0.43099999999999999</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>4</v>
+      </c>
+      <c r="B206" t="s">
+        <v>5</v>
+      </c>
+      <c r="C206">
+        <v>5</v>
+      </c>
+      <c r="D206">
+        <v>0.378</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>4</v>
+      </c>
+      <c r="B207" t="s">
+        <v>6</v>
+      </c>
+      <c r="C207">
+        <v>1</v>
+      </c>
+      <c r="D207">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>4</v>
+      </c>
+      <c r="B208" t="s">
+        <v>6</v>
+      </c>
+      <c r="C208">
+        <v>2</v>
+      </c>
+      <c r="D208">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>4</v>
+      </c>
+      <c r="B209" t="s">
+        <v>6</v>
+      </c>
+      <c r="C209">
+        <v>3</v>
+      </c>
+      <c r="D209">
+        <v>0.63100000000000001</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>4</v>
+      </c>
+      <c r="B210" t="s">
+        <v>6</v>
+      </c>
+      <c r="C210">
+        <v>4</v>
+      </c>
+      <c r="D210">
+        <v>0.49099999999999999</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>4</v>
+      </c>
+      <c r="B211" t="s">
+        <v>6</v>
+      </c>
+      <c r="C211">
+        <v>5</v>
+      </c>
+      <c r="D211">
+        <v>0.44600000000000001</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>7</v>
+      </c>
+      <c r="B212" t="s">
+        <v>5</v>
+      </c>
+      <c r="C212">
+        <v>1</v>
+      </c>
+      <c r="D212">
+        <v>0.46300000000000002</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>7</v>
+      </c>
+      <c r="B213" t="s">
+        <v>5</v>
+      </c>
+      <c r="C213">
+        <v>2</v>
+      </c>
+      <c r="D213">
+        <v>0.23899999999999999</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>7</v>
+      </c>
+      <c r="B214" t="s">
+        <v>5</v>
+      </c>
+      <c r="C214">
+        <v>3</v>
+      </c>
+      <c r="D214">
+        <v>0.41199999999999998</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>7</v>
+      </c>
+      <c r="B215" t="s">
+        <v>5</v>
+      </c>
+      <c r="C215">
+        <v>4</v>
+      </c>
+      <c r="D215">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>7</v>
+      </c>
+      <c r="B216" t="s">
+        <v>5</v>
+      </c>
+      <c r="C216">
+        <v>5</v>
+      </c>
+      <c r="D216">
+        <v>0.28799999999999998</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>7</v>
+      </c>
+      <c r="B217" t="s">
+        <v>6</v>
+      </c>
+      <c r="C217">
+        <v>1</v>
+      </c>
+      <c r="D217">
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>7</v>
+      </c>
+      <c r="B218" t="s">
+        <v>6</v>
+      </c>
+      <c r="C218">
+        <v>2</v>
+      </c>
+      <c r="D218">
+        <v>0.54400000000000004</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>7</v>
+      </c>
+      <c r="B219" t="s">
+        <v>6</v>
+      </c>
+      <c r="C219">
+        <v>3</v>
+      </c>
+      <c r="D219">
+        <v>0.51500000000000001</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>7</v>
+      </c>
+      <c r="B220" t="s">
+        <v>6</v>
+      </c>
+      <c r="C220">
+        <v>4</v>
+      </c>
+      <c r="D220">
+        <v>0.68400000000000005</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>7</v>
+      </c>
+      <c r="B221" t="s">
+        <v>6</v>
+      </c>
+      <c r="C221">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>